<commit_message>
Update with restock suggestion
</commit_message>
<xml_diff>
--- a/Sufficient data WITH_PO/forecast_summary_B07GBM3M88_WITH_PO.xlsx
+++ b/Sufficient data WITH_PO/forecast_summary_B07GBM3M88_WITH_PO.xlsx
@@ -414,7 +414,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R17"/>
+  <dimension ref="A1:Q17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -505,11 +505,6 @@
       </c>
       <c r="Q1" t="inlineStr">
         <is>
-          <t>Sales Volume Rank</t>
-        </is>
-      </c>
-      <c r="R1" t="inlineStr">
-        <is>
           <t>Lifecycle Stage</t>
         </is>
       </c>
@@ -520,7 +515,11 @@
           <t>W1</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr"/>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>2025-02-02</t>
+        </is>
+      </c>
       <c r="C2" t="inlineStr">
         <is>
           <t>B07GBM3M88</t>
@@ -553,7 +552,7 @@
         </is>
       </c>
       <c r="L2" t="n">
-        <v>14.4</v>
+        <v>14.42</v>
       </c>
       <c r="M2" t="inlineStr">
         <is>
@@ -571,14 +570,11 @@
         </is>
       </c>
       <c r="P2" t="n">
-        <v>1.08</v>
-      </c>
-      <c r="Q2" t="n">
-        <v>14</v>
-      </c>
-      <c r="R2" t="inlineStr">
-        <is>
-          <t>Growth</t>
+        <v>0.9399999999999999</v>
+      </c>
+      <c r="Q2" t="inlineStr">
+        <is>
+          <t>Mature</t>
         </is>
       </c>
     </row>
@@ -588,7 +584,11 @@
           <t>W2</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr"/>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>2025-02-09</t>
+        </is>
+      </c>
       <c r="C3" t="inlineStr">
         <is>
           <t>B07GBM3M88</t>
@@ -621,7 +621,7 @@
         </is>
       </c>
       <c r="L3" t="n">
-        <v>14.4</v>
+        <v>13.42</v>
       </c>
       <c r="M3" t="inlineStr">
         <is>
@@ -639,14 +639,11 @@
         </is>
       </c>
       <c r="P3" t="n">
-        <v>1.18</v>
-      </c>
-      <c r="Q3" t="n">
-        <v>14</v>
-      </c>
-      <c r="R3" t="inlineStr">
-        <is>
-          <t>Growth</t>
+        <v>0.98</v>
+      </c>
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t>Mature</t>
         </is>
       </c>
     </row>
@@ -656,7 +653,11 @@
           <t>W3</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr"/>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>2025-02-16</t>
+        </is>
+      </c>
       <c r="C4" t="inlineStr">
         <is>
           <t>B07GBM3M88</t>
@@ -689,7 +690,7 @@
         </is>
       </c>
       <c r="L4" t="n">
-        <v>14.4</v>
+        <v>12.42</v>
       </c>
       <c r="M4" t="inlineStr">
         <is>
@@ -707,14 +708,11 @@
         </is>
       </c>
       <c r="P4" t="n">
-        <v>1.18</v>
-      </c>
-      <c r="Q4" t="n">
-        <v>14</v>
-      </c>
-      <c r="R4" t="inlineStr">
-        <is>
-          <t>Growth</t>
+        <v>0.9</v>
+      </c>
+      <c r="Q4" t="inlineStr">
+        <is>
+          <t>Mature</t>
         </is>
       </c>
     </row>
@@ -724,7 +722,11 @@
           <t>W4</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr"/>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>2025-02-23</t>
+        </is>
+      </c>
       <c r="C5" t="inlineStr">
         <is>
           <t>B07GBM3M88</t>
@@ -757,7 +759,7 @@
         </is>
       </c>
       <c r="L5" t="n">
-        <v>14.4</v>
+        <v>11.42</v>
       </c>
       <c r="M5" t="inlineStr">
         <is>
@@ -775,14 +777,11 @@
         </is>
       </c>
       <c r="P5" t="n">
-        <v>1.13</v>
-      </c>
-      <c r="Q5" t="n">
-        <v>14</v>
-      </c>
-      <c r="R5" t="inlineStr">
-        <is>
-          <t>Growth</t>
+        <v>0.9399999999999999</v>
+      </c>
+      <c r="Q5" t="inlineStr">
+        <is>
+          <t>Mature</t>
         </is>
       </c>
     </row>
@@ -792,7 +791,11 @@
           <t>W5</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr"/>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>2025-03-02</t>
+        </is>
+      </c>
       <c r="C6" t="inlineStr">
         <is>
           <t>B07GBM3M88</t>
@@ -825,7 +828,7 @@
         </is>
       </c>
       <c r="L6" t="n">
-        <v>14.4</v>
+        <v>10.42</v>
       </c>
       <c r="M6" t="inlineStr">
         <is>
@@ -843,14 +846,11 @@
         </is>
       </c>
       <c r="P6" t="n">
-        <v>0.91</v>
-      </c>
-      <c r="Q6" t="n">
-        <v>14</v>
-      </c>
-      <c r="R6" t="inlineStr">
-        <is>
-          <t>Growth</t>
+        <v>0.88</v>
+      </c>
+      <c r="Q6" t="inlineStr">
+        <is>
+          <t>Mature</t>
         </is>
       </c>
     </row>
@@ -860,7 +860,11 @@
           <t>W6</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr"/>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>2025-03-09</t>
+        </is>
+      </c>
       <c r="C7" t="inlineStr">
         <is>
           <t>B07GBM3M88</t>
@@ -893,7 +897,7 @@
         </is>
       </c>
       <c r="L7" t="n">
-        <v>14.4</v>
+        <v>9.42</v>
       </c>
       <c r="M7" t="inlineStr">
         <is>
@@ -911,14 +915,11 @@
         </is>
       </c>
       <c r="P7" t="n">
-        <v>1.01</v>
-      </c>
-      <c r="Q7" t="n">
-        <v>14</v>
-      </c>
-      <c r="R7" t="inlineStr">
-        <is>
-          <t>Growth</t>
+        <v>0.9</v>
+      </c>
+      <c r="Q7" t="inlineStr">
+        <is>
+          <t>Mature</t>
         </is>
       </c>
     </row>
@@ -928,7 +929,11 @@
           <t>W7</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr"/>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>2025-03-16</t>
+        </is>
+      </c>
       <c r="C8" t="inlineStr">
         <is>
           <t>B07GBM3M88</t>
@@ -961,7 +966,7 @@
         </is>
       </c>
       <c r="L8" t="n">
-        <v>14.4</v>
+        <v>8.42</v>
       </c>
       <c r="M8" t="inlineStr">
         <is>
@@ -979,14 +984,11 @@
         </is>
       </c>
       <c r="P8" t="n">
-        <v>0.86</v>
-      </c>
-      <c r="Q8" t="n">
-        <v>14</v>
-      </c>
-      <c r="R8" t="inlineStr">
-        <is>
-          <t>Growth</t>
+        <v>0.8</v>
+      </c>
+      <c r="Q8" t="inlineStr">
+        <is>
+          <t>Mature</t>
         </is>
       </c>
     </row>
@@ -996,7 +998,11 @@
           <t>W8</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr"/>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>2025-03-23</t>
+        </is>
+      </c>
       <c r="C9" t="inlineStr">
         <is>
           <t>B07GBM3M88</t>
@@ -1029,7 +1035,7 @@
         </is>
       </c>
       <c r="L9" t="n">
-        <v>14.4</v>
+        <v>7.42</v>
       </c>
       <c r="M9" t="inlineStr">
         <is>
@@ -1047,14 +1053,11 @@
         </is>
       </c>
       <c r="P9" t="n">
-        <v>1.02</v>
-      </c>
-      <c r="Q9" t="n">
-        <v>14</v>
-      </c>
-      <c r="R9" t="inlineStr">
-        <is>
-          <t>Growth</t>
+        <v>1.18</v>
+      </c>
+      <c r="Q9" t="inlineStr">
+        <is>
+          <t>Mature</t>
         </is>
       </c>
     </row>
@@ -1064,7 +1067,11 @@
           <t>W9</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr"/>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>2025-03-30</t>
+        </is>
+      </c>
       <c r="C10" t="inlineStr">
         <is>
           <t>B07GBM3M88</t>
@@ -1097,7 +1104,7 @@
         </is>
       </c>
       <c r="L10" t="n">
-        <v>14.4</v>
+        <v>6.42</v>
       </c>
       <c r="M10" t="inlineStr">
         <is>
@@ -1115,14 +1122,11 @@
         </is>
       </c>
       <c r="P10" t="n">
-        <v>0.92</v>
-      </c>
-      <c r="Q10" t="n">
-        <v>14</v>
-      </c>
-      <c r="R10" t="inlineStr">
-        <is>
-          <t>Growth</t>
+        <v>0.88</v>
+      </c>
+      <c r="Q10" t="inlineStr">
+        <is>
+          <t>Mature</t>
         </is>
       </c>
     </row>
@@ -1132,7 +1136,11 @@
           <t>W10</t>
         </is>
       </c>
-      <c r="B11" t="inlineStr"/>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>2025-04-06</t>
+        </is>
+      </c>
       <c r="C11" t="inlineStr">
         <is>
           <t>B07GBM3M88</t>
@@ -1165,7 +1173,7 @@
         </is>
       </c>
       <c r="L11" t="n">
-        <v>14.4</v>
+        <v>5.42</v>
       </c>
       <c r="M11" t="inlineStr">
         <is>
@@ -1183,14 +1191,11 @@
         </is>
       </c>
       <c r="P11" t="n">
-        <v>0.88</v>
-      </c>
-      <c r="Q11" t="n">
-        <v>14</v>
-      </c>
-      <c r="R11" t="inlineStr">
-        <is>
-          <t>Growth</t>
+        <v>1.19</v>
+      </c>
+      <c r="Q11" t="inlineStr">
+        <is>
+          <t>Mature</t>
         </is>
       </c>
     </row>
@@ -1200,7 +1205,11 @@
           <t>W11</t>
         </is>
       </c>
-      <c r="B12" t="inlineStr"/>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>2025-04-13</t>
+        </is>
+      </c>
       <c r="C12" t="inlineStr">
         <is>
           <t>B07GBM3M88</t>
@@ -1233,7 +1242,7 @@
         </is>
       </c>
       <c r="L12" t="n">
-        <v>14.4</v>
+        <v>4.42</v>
       </c>
       <c r="M12" t="inlineStr">
         <is>
@@ -1251,14 +1260,11 @@
         </is>
       </c>
       <c r="P12" t="n">
-        <v>1.04</v>
-      </c>
-      <c r="Q12" t="n">
-        <v>14</v>
-      </c>
-      <c r="R12" t="inlineStr">
-        <is>
-          <t>Growth</t>
+        <v>1.17</v>
+      </c>
+      <c r="Q12" t="inlineStr">
+        <is>
+          <t>Mature</t>
         </is>
       </c>
     </row>
@@ -1268,7 +1274,11 @@
           <t>W12</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr"/>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>2025-04-20</t>
+        </is>
+      </c>
       <c r="C13" t="inlineStr">
         <is>
           <t>B07GBM3M88</t>
@@ -1301,7 +1311,7 @@
         </is>
       </c>
       <c r="L13" t="n">
-        <v>14.4</v>
+        <v>3.42</v>
       </c>
       <c r="M13" t="inlineStr">
         <is>
@@ -1319,14 +1329,11 @@
         </is>
       </c>
       <c r="P13" t="n">
-        <v>0.98</v>
-      </c>
-      <c r="Q13" t="n">
-        <v>14</v>
-      </c>
-      <c r="R13" t="inlineStr">
-        <is>
-          <t>Growth</t>
+        <v>0.96</v>
+      </c>
+      <c r="Q13" t="inlineStr">
+        <is>
+          <t>Mature</t>
         </is>
       </c>
     </row>
@@ -1336,7 +1343,11 @@
           <t>W13</t>
         </is>
       </c>
-      <c r="B14" t="inlineStr"/>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>2025-04-27</t>
+        </is>
+      </c>
       <c r="C14" t="inlineStr">
         <is>
           <t>B07GBM3M88</t>
@@ -1369,7 +1380,7 @@
         </is>
       </c>
       <c r="L14" t="n">
-        <v>14.4</v>
+        <v>2.42</v>
       </c>
       <c r="M14" t="inlineStr">
         <is>
@@ -1387,14 +1398,11 @@
         </is>
       </c>
       <c r="P14" t="n">
-        <v>1.17</v>
-      </c>
-      <c r="Q14" t="n">
-        <v>14</v>
-      </c>
-      <c r="R14" t="inlineStr">
-        <is>
-          <t>Growth</t>
+        <v>0.85</v>
+      </c>
+      <c r="Q14" t="inlineStr">
+        <is>
+          <t>Mature</t>
         </is>
       </c>
     </row>
@@ -1404,7 +1412,11 @@
           <t>W14</t>
         </is>
       </c>
-      <c r="B15" t="inlineStr"/>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>2025-05-04</t>
+        </is>
+      </c>
       <c r="C15" t="inlineStr">
         <is>
           <t>B07GBM3M88</t>
@@ -1437,7 +1449,7 @@
         </is>
       </c>
       <c r="L15" t="n">
-        <v>14.4</v>
+        <v>1.42</v>
       </c>
       <c r="M15" t="inlineStr">
         <is>
@@ -1455,14 +1467,11 @@
         </is>
       </c>
       <c r="P15" t="n">
-        <v>0.84</v>
-      </c>
-      <c r="Q15" t="n">
-        <v>14</v>
-      </c>
-      <c r="R15" t="inlineStr">
-        <is>
-          <t>Growth</t>
+        <v>1.02</v>
+      </c>
+      <c r="Q15" t="inlineStr">
+        <is>
+          <t>Mature</t>
         </is>
       </c>
     </row>
@@ -1472,7 +1481,11 @@
           <t>W15</t>
         </is>
       </c>
-      <c r="B16" t="inlineStr"/>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>2025-05-11</t>
+        </is>
+      </c>
       <c r="C16" t="inlineStr">
         <is>
           <t>B07GBM3M88</t>
@@ -1505,16 +1518,16 @@
         </is>
       </c>
       <c r="L16" t="n">
-        <v>14.4</v>
+        <v>0.42</v>
       </c>
       <c r="M16" t="inlineStr">
         <is>
-          <t>Low</t>
+          <t>High</t>
         </is>
       </c>
       <c r="N16" t="inlineStr">
         <is>
-          <t>Normal</t>
+          <t>Urgent</t>
         </is>
       </c>
       <c r="O16" t="inlineStr">
@@ -1523,14 +1536,11 @@
         </is>
       </c>
       <c r="P16" t="n">
-        <v>1.02</v>
-      </c>
-      <c r="Q16" t="n">
-        <v>14</v>
-      </c>
-      <c r="R16" t="inlineStr">
-        <is>
-          <t>Growth</t>
+        <v>1.17</v>
+      </c>
+      <c r="Q16" t="inlineStr">
+        <is>
+          <t>Mature</t>
         </is>
       </c>
     </row>
@@ -1540,7 +1550,11 @@
           <t>W16</t>
         </is>
       </c>
-      <c r="B17" t="inlineStr"/>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>2025-05-18</t>
+        </is>
+      </c>
       <c r="C17" t="inlineStr">
         <is>
           <t>B07GBM3M88</t>
@@ -1573,16 +1587,16 @@
         </is>
       </c>
       <c r="L17" t="n">
-        <v>14.4</v>
+        <v>0</v>
       </c>
       <c r="M17" t="inlineStr">
         <is>
-          <t>Low</t>
+          <t>High</t>
         </is>
       </c>
       <c r="N17" t="inlineStr">
         <is>
-          <t>Normal</t>
+          <t>Urgent</t>
         </is>
       </c>
       <c r="O17" t="inlineStr">
@@ -1591,14 +1605,11 @@
         </is>
       </c>
       <c r="P17" t="n">
-        <v>1.17</v>
-      </c>
-      <c r="Q17" t="n">
-        <v>14</v>
-      </c>
-      <c r="R17" t="inlineStr">
-        <is>
-          <t>Growth</t>
+        <v>0.9</v>
+      </c>
+      <c r="Q17" t="inlineStr">
+        <is>
+          <t>Mature</t>
         </is>
       </c>
     </row>
@@ -1773,7 +1784,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>2025-02-02</t>
+          <t>N/A</t>
         </is>
       </c>
     </row>
@@ -1797,7 +1808,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>2025-02-02</t>
+          <t>N/A</t>
         </is>
       </c>
     </row>

</xml_diff>